<commit_message>
Hotfix - Kantinenarbeiter isn't able to order anymore
</commit_message>
<xml_diff>
--- a/Dokumentation/Rollenmodell.xlsx
+++ b/Dokumentation/Rollenmodell.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitProjekte\Kantinerado\Dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9445A1C0-B3D4-43B0-84F8-62EBE35FF819}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{598A21E9-7BA0-4F59-B481-6200EB27D098}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1068" yWindow="-108" windowWidth="22080" windowHeight="13176" xr2:uid="{432ED4F4-662B-4FAD-B55E-CEF03951BEEB}"/>
+    <workbookView xWindow="1020" yWindow="-108" windowWidth="22128" windowHeight="13176" xr2:uid="{432ED4F4-662B-4FAD-B55E-CEF03951BEEB}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="25">
   <si>
     <t>Rollenkonzept</t>
   </si>
@@ -75,9 +75,6 @@
   </si>
   <si>
     <t>Preis</t>
-  </si>
-  <si>
-    <t>Reduziert</t>
   </si>
   <si>
     <t xml:space="preserve">Normal </t>
@@ -582,8 +579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9FAFE9C-36FC-4308-9922-4A6769DEBA34}">
   <dimension ref="B2:O10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="149" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="149" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -632,7 +629,7 @@
         <v>6</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>11</v>
@@ -641,31 +638,31 @@
         <v>12</v>
       </c>
       <c r="G6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="H6" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J6" s="5" t="s">
+      <c r="K6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="M6" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="K6" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="L6" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="M6" s="5" t="s">
+      <c r="N6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="N6" s="5" t="s">
+      <c r="O6" s="5" t="s">
         <v>24</v>
-      </c>
-      <c r="O6" s="5" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.3">
@@ -726,7 +723,7 @@
         <v>9</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>9</v>
@@ -770,7 +767,7 @@
         <v>9</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>8</v>

</xml_diff>